<commit_message>
Refactor item spawning logic and add default values to Item properties
</commit_message>
<xml_diff>
--- a/SpawnProbabilityDictionaryGenerator.xlsx
+++ b/SpawnProbabilityDictionaryGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darius Rohde\AppData\LocalLow\melodymania\Melody Mania\Mods\ItemRumbleMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07E3F39-0C2A-435D-9B58-37B0B1F08B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37907066-A551-4CF5-AE32-E88D7028BFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{950D2CEC-F685-4FB6-B45D-6FBBFAD69F2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{950D2CEC-F685-4FB6-B45D-6FBBFAD69F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -411,16 +411,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A13505-FC75-4C80-ACC8-831FF76A0D8B}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="15" max="15" width="35.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" customWidth="1"/>
     <col min="17" max="17" width="15.85546875" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" customWidth="1"/>
   </cols>
@@ -455,10 +455,10 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O2">
         <f>SUM(B2:N2)</f>
@@ -466,11 +466,11 @@
       </c>
       <c r="Q2" t="str">
         <f>CONCATENATE("{",$A2,", ",B2,"}")</f>
-        <v>{100, 100}</v>
+        <v>{100, 0}</v>
       </c>
       <c r="R2" t="str">
         <f>CONCATENATE("{",$A2,", ",C2,"}")</f>
-        <v>{100, 100}</v>
+        <v>{100, 200}</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -478,10 +478,10 @@
         <v>150</v>
       </c>
       <c r="B3">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O17" si="0">SUM(B3:N3)</f>
@@ -489,11 +489,11 @@
       </c>
       <c r="Q3" t="str">
         <f t="shared" ref="Q3:R17" si="1">CONCATENATE("{",$A3,", ",B3,"}")</f>
-        <v>{150, 105}</v>
+        <v>{150, 0}</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="1"/>
-        <v>{150, 95}</v>
+        <v>{150, 200}</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -501,10 +501,10 @@
         <v>200</v>
       </c>
       <c r="B4">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
@@ -512,11 +512,11 @@
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="1"/>
-        <v>{200, 110}</v>
+        <v>{200, 0}</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="1"/>
-        <v>{200, 90}</v>
+        <v>{200, 200}</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -524,10 +524,10 @@
         <v>250</v>
       </c>
       <c r="B5">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
@@ -535,11 +535,11 @@
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="1"/>
-        <v>{250, 115}</v>
+        <v>{250, 0}</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="1"/>
-        <v>{250, 85}</v>
+        <v>{250, 200}</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -547,10 +547,10 @@
         <v>300</v>
       </c>
       <c r="B6">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
@@ -558,11 +558,11 @@
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="1"/>
-        <v>{300, 120}</v>
+        <v>{300, 0}</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="1"/>
-        <v>{300, 80}</v>
+        <v>{300, 200}</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -570,10 +570,10 @@
         <v>350</v>
       </c>
       <c r="B7">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
@@ -581,11 +581,11 @@
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="1"/>
-        <v>{350, 125}</v>
+        <v>{350, 0}</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="1"/>
-        <v>{350, 75}</v>
+        <v>{350, 200}</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -593,10 +593,10 @@
         <v>400</v>
       </c>
       <c r="B8">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
@@ -604,11 +604,11 @@
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="1"/>
-        <v>{400, 130}</v>
+        <v>{400, 0}</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="1"/>
-        <v>{400, 70}</v>
+        <v>{400, 200}</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -616,10 +616,10 @@
         <v>450</v>
       </c>
       <c r="B9">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>65</v>
+        <v>200</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
@@ -627,11 +627,11 @@
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="1"/>
-        <v>{450, 135}</v>
+        <v>{450, 0}</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="1"/>
-        <v>{450, 65}</v>
+        <v>{450, 200}</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -639,10 +639,10 @@
         <v>500</v>
       </c>
       <c r="B10">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
@@ -650,11 +650,11 @@
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="1"/>
-        <v>{500, 140}</v>
+        <v>{500, 0}</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="1"/>
-        <v>{500, 60}</v>
+        <v>{500, 200}</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>550</v>
       </c>
       <c r="B11">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
@@ -673,11 +673,11 @@
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="1"/>
-        <v>{550, 145}</v>
+        <v>{550, 0}</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" si="1"/>
-        <v>{550, 55}</v>
+        <v>{550, 200}</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -685,10 +685,10 @@
         <v>600</v>
       </c>
       <c r="B12">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="O12">
         <f t="shared" si="0"/>
@@ -696,11 +696,11 @@
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="1"/>
-        <v>{600, 150}</v>
+        <v>{600, 0}</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="1"/>
-        <v>{600, 50}</v>
+        <v>{600, 200}</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -708,10 +708,10 @@
         <v>650</v>
       </c>
       <c r="B13">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
@@ -719,11 +719,11 @@
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="1"/>
-        <v>{650, 155}</v>
+        <v>{650, 0}</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="1"/>
-        <v>{650, 45}</v>
+        <v>{650, 200}</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -731,10 +731,10 @@
         <v>700</v>
       </c>
       <c r="B14">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
@@ -742,11 +742,11 @@
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="1"/>
-        <v>{700, 160}</v>
+        <v>{700, 0}</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" si="1"/>
-        <v>{700, 40}</v>
+        <v>{700, 200}</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -754,10 +754,10 @@
         <v>750</v>
       </c>
       <c r="B15">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
@@ -765,11 +765,11 @@
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="1"/>
-        <v>{750, 165}</v>
+        <v>{750, 0}</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="1"/>
-        <v>{750, 35}</v>
+        <v>{750, 200}</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -777,10 +777,10 @@
         <v>800</v>
       </c>
       <c r="B16">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="O16">
         <f t="shared" si="0"/>
@@ -788,11 +788,11 @@
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="1"/>
-        <v>{800, 170}</v>
+        <v>{800, 0}</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="1"/>
-        <v>{800, 30}</v>
+        <v>{800, 200}</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -800,10 +800,10 @@
         <v>1000</v>
       </c>
       <c r="B17">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O17">
         <f t="shared" si="0"/>
@@ -811,11 +811,11 @@
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="1"/>
+        <v>{1000, 0}</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="1"/>
         <v>{1000, 200}</v>
-      </c>
-      <c r="R17" t="str">
-        <f t="shared" si="1"/>
-        <v>{1000, 0}</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -883,11 +883,11 @@
       </c>
       <c r="B24" s="1" t="str">
         <f>CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", Q2:Q17),"}")</f>
-        <v>{{100, 100}, {150, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {1000, 200}}</v>
+        <v>{{100, 0}, {150, 0}, {200, 0}, {250, 0}, {300, 0}, {350, 0}, {400, 0}, {450, 0}, {500, 0}, {550, 0}, {600, 0}, {650, 0}, {700, 0}, {750, 0}, {800, 0}, {1000, 0}}</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", R2:R17),"}")</f>
-        <v>{{100, 100}, {150, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 40}, {750, 35}, {800, 30}, {1000, 0}}</v>
+        <v>{{100, 200}, {150, 200}, {200, 200}, {250, 200}, {300, 200}, {350, 200}, {400, 200}, {450, 200}, {500, 200}, {550, 200}, {600, 200}, {650, 200}, {700, 200}, {750, 200}, {800, 200}, {1000, 200}}</v>
       </c>
       <c r="D24" s="1" t="str">
         <f t="shared" ref="D24:N24" si="3">CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", S2:S17),"}")</f>
@@ -932,6 +932,134 @@
       <c r="N24" s="1" t="str">
         <f t="shared" si="3"/>
         <v>{, , , , , , , , , , , , , , , }</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>100</v>
+      </c>
+      <c r="D56">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>105</v>
+      </c>
+      <c r="D57">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>110</v>
+      </c>
+      <c r="D58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>115</v>
+      </c>
+      <c r="D59">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>120</v>
+      </c>
+      <c r="D60">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>125</v>
+      </c>
+      <c r="D61">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>130</v>
+      </c>
+      <c r="D62">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>135</v>
+      </c>
+      <c r="D63">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>140</v>
+      </c>
+      <c r="D64">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>145</v>
+      </c>
+      <c r="D65">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>150</v>
+      </c>
+      <c r="D66">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>155</v>
+      </c>
+      <c r="D67">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>160</v>
+      </c>
+      <c r="D68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>165</v>
+      </c>
+      <c r="D69">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>170</v>
+      </c>
+      <c r="D70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new methods to ItemActions class
</commit_message>
<xml_diff>
--- a/SpawnProbabilityDictionaryGenerator.xlsx
+++ b/SpawnProbabilityDictionaryGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darius Rohde\AppData\LocalLow\melodymania\Melody Mania\Mods\ItemRumbleMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485026E8-17D0-407D-8E82-0E8A435E002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999036C5-FFC3-4C41-A98A-B00BF366AEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{950D2CEC-F685-4FB6-B45D-6FBBFAD69F2F}"/>
   </bookViews>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A13505-FC75-4C80-ACC8-831FF76A0D8B}">
   <dimension ref="A1:Z92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,10 +571,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -586,19 +586,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H2" s="3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
       <c r="J2" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K2" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -606,15 +606,15 @@
       <c r="O2" s="3"/>
       <c r="P2">
         <f>SUM(B2:O2)</f>
-        <v>70</v>
+        <v>226</v>
       </c>
       <c r="Q2" t="str">
         <f>CONCATENATE("{",$A2,", ",B2,"}")</f>
-        <v>{0, 10}</v>
+        <v>{0, 80}</v>
       </c>
       <c r="R2" t="str">
         <f>CONCATENATE("{",$A2,", ",C2,"}")</f>
-        <v>{0, 50}</v>
+        <v>{0, 90}</v>
       </c>
       <c r="S2" t="str">
         <f t="shared" ref="S2:U17" si="1">CONCATENATE("{",$A2,", ",D2,"}")</f>
@@ -630,11 +630,11 @@
       </c>
       <c r="V2" t="str">
         <f t="shared" ref="V2:V40" si="2">CONCATENATE("{",$A2,", ",G2,"}")</f>
-        <v>{0, 2}</v>
+        <v>{0, 20}</v>
       </c>
       <c r="W2" t="str">
         <f t="shared" ref="W2:W40" si="3">CONCATENATE("{",$A2,", ",H2,"}")</f>
-        <v>{0, 2}</v>
+        <v>{0, 20}</v>
       </c>
       <c r="X2" t="str">
         <f t="shared" ref="X2:X40" si="4">CONCATENATE("{",$A2,", ",I2,"}")</f>
@@ -642,11 +642,11 @@
       </c>
       <c r="Y2" t="str">
         <f t="shared" ref="Y2:Y40" si="5">CONCATENATE("{",$A2,", ",J2,"}")</f>
-        <v>{0, 0}</v>
+        <v>{0, 5}</v>
       </c>
       <c r="Z2" t="str">
         <f t="shared" ref="Z2:AA40" si="6">CONCATENATE("{",$A2,", ",K2,"}")</f>
-        <v>{0, 0}</v>
+        <v>{0, 5}</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K3" s="3">
         <v>10</v>
@@ -689,7 +689,7 @@
       <c r="O3" s="3"/>
       <c r="P3">
         <f t="shared" ref="P3:P40" si="7">SUM(B3:O3)</f>
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" ref="Q3:R17" si="8">CONCATENATE("{",$A3,", ",B3,"}")</f>
@@ -725,7 +725,7 @@
       </c>
       <c r="Y3" t="str">
         <f t="shared" si="5"/>
-        <v>{10, 2}</v>
+        <v>{10, 10}</v>
       </c>
       <c r="Z3" t="str">
         <f t="shared" si="6"/>
@@ -761,10 +761,10 @@
         <v>39</v>
       </c>
       <c r="J4" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K4" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -772,7 +772,7 @@
       <c r="O4" s="3"/>
       <c r="P4">
         <f t="shared" si="7"/>
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="8"/>
@@ -808,11 +808,11 @@
       </c>
       <c r="Y4" t="str">
         <f t="shared" si="5"/>
-        <v>{200, 1}</v>
+        <v>{200, 10}</v>
       </c>
       <c r="Z4" t="str">
         <f t="shared" si="6"/>
-        <v>{200, 1}</v>
+        <v>{200, 10}</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -844,10 +844,10 @@
         <v>58</v>
       </c>
       <c r="J5" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K5" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -855,7 +855,7 @@
       <c r="O5" s="3"/>
       <c r="P5">
         <f t="shared" si="7"/>
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="8"/>
@@ -891,11 +891,11 @@
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="5"/>
-        <v>{250, 1}</v>
+        <v>{250, 10}</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="6"/>
-        <v>{250, 1}</v>
+        <v>{250, 10}</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -927,10 +927,10 @@
         <v>58</v>
       </c>
       <c r="J6" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K6" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -938,7 +938,7 @@
       <c r="O6" s="3"/>
       <c r="P6">
         <f t="shared" si="7"/>
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="8"/>
@@ -974,11 +974,11 @@
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="5"/>
-        <v>{300, 1}</v>
+        <v>{300, 10}</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="6"/>
-        <v>{300, 1}</v>
+        <v>{300, 10}</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1010,10 +1010,10 @@
         <v>58</v>
       </c>
       <c r="J7" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K7" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1021,7 +1021,7 @@
       <c r="O7" s="3"/>
       <c r="P7">
         <f t="shared" si="7"/>
-        <v>394</v>
+        <v>412</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="8"/>
@@ -1057,11 +1057,11 @@
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="5"/>
-        <v>{350, 1}</v>
+        <v>{350, 10}</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="6"/>
-        <v>{350, 1}</v>
+        <v>{350, 10}</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1093,10 +1093,10 @@
         <v>58</v>
       </c>
       <c r="J8" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K8" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1104,7 +1104,7 @@
       <c r="O8" s="3"/>
       <c r="P8">
         <f t="shared" si="7"/>
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="8"/>
@@ -1140,11 +1140,11 @@
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="5"/>
-        <v>{400, 1}</v>
+        <v>{400, 10}</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="6"/>
-        <v>{400, 1}</v>
+        <v>{400, 10}</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1176,10 +1176,10 @@
         <v>58</v>
       </c>
       <c r="J9" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K9" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1187,7 +1187,7 @@
       <c r="O9" s="3"/>
       <c r="P9">
         <f t="shared" si="7"/>
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="8"/>
@@ -1223,11 +1223,11 @@
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="5"/>
-        <v>{450, 1}</v>
+        <v>{450, 10}</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="6"/>
-        <v>{450, 1}</v>
+        <v>{450, 10}</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H12" s="3">
         <v>26</v>
@@ -1436,7 +1436,7 @@
       <c r="O12" s="3"/>
       <c r="P12">
         <f t="shared" si="7"/>
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="8"/>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="V12" t="str">
         <f t="shared" si="2"/>
-        <v>{600, 20}</v>
+        <v>{600, 100}</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="3"/>
@@ -1496,10 +1496,10 @@
         <v>20</v>
       </c>
       <c r="F13" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G13" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H13" s="3">
         <v>26</v>
@@ -1519,7 +1519,7 @@
       <c r="O13" s="3"/>
       <c r="P13">
         <f t="shared" si="7"/>
-        <v>412</v>
+        <v>524</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="8"/>
@@ -1539,11 +1539,11 @@
       </c>
       <c r="U13" t="str">
         <f t="shared" si="1"/>
-        <v>{650, 18}</v>
+        <v>{650, 50}</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="2"/>
-        <v>{650, 20}</v>
+        <v>{650, 100}</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="3"/>
@@ -1570,7 +1570,7 @@
         <v>160</v>
       </c>
       <c r="C14" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3">
         <v>22</v>
@@ -1579,10 +1579,10 @@
         <v>20</v>
       </c>
       <c r="F14" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G14" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H14" s="3">
         <v>26</v>
@@ -1602,7 +1602,7 @@
       <c r="O14" s="3"/>
       <c r="P14">
         <f t="shared" si="7"/>
-        <v>414</v>
+        <v>531</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="8"/>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="8"/>
-        <v>{700, 40}</v>
+        <v>{700, 45}</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="1"/>
@@ -1622,11 +1622,11 @@
       </c>
       <c r="U14" t="str">
         <f t="shared" si="1"/>
-        <v>{700, 18}</v>
+        <v>{700, 50}</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="2"/>
-        <v>{700, 20}</v>
+        <v>{700, 100}</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="3"/>
@@ -1653,7 +1653,7 @@
         <v>165</v>
       </c>
       <c r="C15" s="3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3">
         <v>24</v>
@@ -1662,10 +1662,10 @@
         <v>20</v>
       </c>
       <c r="F15" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H15" s="3">
         <v>26</v>
@@ -1685,7 +1685,7 @@
       <c r="O15" s="3"/>
       <c r="P15">
         <f t="shared" si="7"/>
-        <v>416</v>
+        <v>538</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="8"/>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="R15" t="str">
         <f t="shared" si="8"/>
-        <v>{750, 35}</v>
+        <v>{750, 45}</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="1"/>
@@ -1705,11 +1705,11 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="1"/>
-        <v>{750, 18}</v>
+        <v>{750, 50}</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="2"/>
-        <v>{750, 20}</v>
+        <v>{750, 100}</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="3"/>
@@ -1736,7 +1736,7 @@
         <v>170</v>
       </c>
       <c r="C16" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D16" s="3">
         <v>26</v>
@@ -1745,7 +1745,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G16" s="3">
         <v>20</v>
@@ -1768,7 +1768,7 @@
       <c r="O16" s="3"/>
       <c r="P16">
         <f t="shared" si="7"/>
-        <v>437</v>
+        <v>484</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="8"/>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="R16" t="str">
         <f t="shared" si="8"/>
-        <v>{800, 30}</v>
+        <v>{800, 45}</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="1"/>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="U16" t="str">
         <f t="shared" si="1"/>
-        <v>{800, 18}</v>
+        <v>{800, 50}</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="2"/>
@@ -1819,7 +1819,7 @@
         <v>170</v>
       </c>
       <c r="C17" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D17" s="3">
         <v>28</v>
@@ -1828,7 +1828,7 @@
         <v>20</v>
       </c>
       <c r="F17" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="G17" s="3">
         <v>20</v>
@@ -1851,7 +1851,7 @@
       <c r="O17" s="3"/>
       <c r="P17">
         <f t="shared" si="7"/>
-        <v>439</v>
+        <v>486</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="8"/>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="8"/>
-        <v>{850, 30}</v>
+        <v>{850, 45}</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="1"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="U17" t="str">
         <f t="shared" si="1"/>
-        <v>{850, 18}</v>
+        <v>{850, 50}</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="2"/>
@@ -1902,7 +1902,7 @@
         <v>171</v>
       </c>
       <c r="C18" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3">
         <v>30</v>
@@ -1911,7 +1911,7 @@
         <v>25</v>
       </c>
       <c r="F18" s="3">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G18" s="3">
         <v>20</v>
@@ -1934,7 +1934,7 @@
       <c r="O18" s="3"/>
       <c r="P18">
         <f t="shared" si="7"/>
-        <v>454</v>
+        <v>494</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" ref="Q18:Q40" si="9">CONCATENATE("{",$A18,", ",B18,"}")</f>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" ref="R18:R40" si="10">CONCATENATE("{",$A18,", ",C18,"}")</f>
-        <v>{900, 30}</v>
+        <v>{900, 45}</v>
       </c>
       <c r="S18" t="str">
         <f t="shared" ref="S18:S40" si="11">CONCATENATE("{",$A18,", ",D18,"}")</f>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="U18" t="str">
         <f t="shared" ref="U18:U40" si="13">CONCATENATE("{",$A18,", ",F18,"}")</f>
-        <v>{900, 25}</v>
+        <v>{900, 50}</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="2"/>
@@ -1985,7 +1985,7 @@
         <v>172</v>
       </c>
       <c r="C19" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3">
         <v>32</v>
@@ -1994,13 +1994,13 @@
         <v>30</v>
       </c>
       <c r="F19" s="3">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3">
         <v>20</v>
       </c>
       <c r="H19" s="3">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="I19" s="3">
         <v>77</v>
@@ -2017,7 +2017,7 @@
       <c r="O19" s="3"/>
       <c r="P19">
         <f t="shared" si="7"/>
-        <v>469</v>
+        <v>576</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="9"/>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="R19" t="str">
         <f t="shared" si="10"/>
-        <v>{950, 30}</v>
+        <v>{950, 45}</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="11"/>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="U19" t="str">
         <f t="shared" si="13"/>
-        <v>{950, 32}</v>
+        <v>{950, 50}</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="2"/>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="W19" t="str">
         <f t="shared" si="3"/>
-        <v>{950, 26}</v>
+        <v>{950, 100}</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="4"/>
@@ -2068,7 +2068,7 @@
         <v>173</v>
       </c>
       <c r="C20" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3">
         <v>34</v>
@@ -2077,13 +2077,13 @@
         <v>35</v>
       </c>
       <c r="F20" s="3">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3">
         <v>20</v>
       </c>
       <c r="H20" s="3">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="I20" s="3">
         <v>77</v>
@@ -2100,7 +2100,7 @@
       <c r="O20" s="3"/>
       <c r="P20">
         <f t="shared" si="7"/>
-        <v>484</v>
+        <v>584</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="9"/>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="10"/>
-        <v>{1000, 30}</v>
+        <v>{1000, 45}</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="11"/>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="U20" t="str">
         <f t="shared" si="13"/>
-        <v>{1000, 39}</v>
+        <v>{1000, 50}</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="2"/>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="W20" t="str">
         <f t="shared" si="3"/>
-        <v>{1000, 26}</v>
+        <v>{1000, 100}</v>
       </c>
       <c r="X20" t="str">
         <f t="shared" si="4"/>
@@ -2151,7 +2151,7 @@
         <v>174</v>
       </c>
       <c r="C21" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D21" s="3">
         <v>36</v>
@@ -2160,13 +2160,13 @@
         <v>40</v>
       </c>
       <c r="F21" s="3">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
       </c>
       <c r="H21" s="3">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="I21" s="3">
         <v>77</v>
@@ -2183,7 +2183,7 @@
       <c r="O21" s="3"/>
       <c r="P21">
         <f t="shared" si="7"/>
-        <v>499</v>
+        <v>592</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="9"/>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="R21" t="str">
         <f t="shared" si="10"/>
-        <v>{1050, 30}</v>
+        <v>{1050, 45}</v>
       </c>
       <c r="S21" t="str">
         <f t="shared" si="11"/>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="U21" t="str">
         <f t="shared" si="13"/>
-        <v>{1050, 46}</v>
+        <v>{1050, 50}</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="2"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="W21" t="str">
         <f t="shared" si="3"/>
-        <v>{1050, 26}</v>
+        <v>{1050, 100}</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" si="4"/>
@@ -2234,7 +2234,7 @@
         <v>175</v>
       </c>
       <c r="C22" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D22" s="3">
         <v>38</v>
@@ -2249,7 +2249,7 @@
         <v>20</v>
       </c>
       <c r="H22" s="3">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="I22" s="3">
         <v>77</v>
@@ -2266,7 +2266,7 @@
       <c r="O22" s="3"/>
       <c r="P22">
         <f t="shared" si="7"/>
-        <v>514</v>
+        <v>603</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="9"/>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="R22" t="str">
         <f t="shared" si="10"/>
-        <v>{1100, 30}</v>
+        <v>{1100, 45}</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="11"/>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="W22" t="str">
         <f t="shared" si="3"/>
-        <v>{1100, 26}</v>
+        <v>{1100, 100}</v>
       </c>
       <c r="X22" t="str">
         <f t="shared" si="4"/>
@@ -2317,7 +2317,7 @@
         <v>176</v>
       </c>
       <c r="C23" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D23" s="3">
         <v>40</v>
@@ -2332,7 +2332,7 @@
         <v>20</v>
       </c>
       <c r="H23" s="3">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="I23" s="3">
         <v>77</v>
@@ -2349,7 +2349,7 @@
       <c r="O23" s="3"/>
       <c r="P23">
         <f t="shared" si="7"/>
-        <v>529</v>
+        <v>618</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="9"/>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="R23" t="str">
         <f t="shared" si="10"/>
-        <v>{1150, 30}</v>
+        <v>{1150, 45}</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="11"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="W23" t="str">
         <f t="shared" si="3"/>
-        <v>{1150, 26}</v>
+        <v>{1150, 100}</v>
       </c>
       <c r="X23" t="str">
         <f t="shared" si="4"/>
@@ -2400,7 +2400,7 @@
         <v>177</v>
       </c>
       <c r="C24" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D24" s="3">
         <v>42</v>
@@ -2432,7 +2432,7 @@
       <c r="O24" s="3"/>
       <c r="P24">
         <f t="shared" si="7"/>
-        <v>544</v>
+        <v>559</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="9"/>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="R24" t="str">
         <f t="shared" si="10"/>
-        <v>{1200, 30}</v>
+        <v>{1200, 45}</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="11"/>
@@ -2483,7 +2483,7 @@
         <v>178</v>
       </c>
       <c r="C25" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D25" s="3">
         <v>44</v>
@@ -2515,7 +2515,7 @@
       <c r="O25" s="3"/>
       <c r="P25">
         <f t="shared" si="7"/>
-        <v>559</v>
+        <v>574</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="9"/>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="R25" t="str">
         <f t="shared" si="10"/>
-        <v>{1250, 30}</v>
+        <v>{1250, 45}</v>
       </c>
       <c r="S25" t="str">
         <f t="shared" si="11"/>
@@ -2566,7 +2566,7 @@
         <v>179</v>
       </c>
       <c r="C26" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D26" s="3">
         <v>46</v>
@@ -2598,7 +2598,7 @@
       <c r="O26" s="3"/>
       <c r="P26">
         <f t="shared" si="7"/>
-        <v>574</v>
+        <v>589</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="9"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="R26" t="str">
         <f t="shared" si="10"/>
-        <v>{1300, 30}</v>
+        <v>{1300, 45}</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" si="11"/>
@@ -2649,7 +2649,7 @@
         <v>180</v>
       </c>
       <c r="C27" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D27" s="4">
         <v>50</v>
@@ -2681,7 +2681,7 @@
       <c r="O27" s="3"/>
       <c r="P27">
         <f t="shared" si="7"/>
-        <v>591</v>
+        <v>606</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="9"/>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="R27" t="str">
         <f t="shared" si="10"/>
-        <v>{1350, 30}</v>
+        <v>{1350, 45}</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="11"/>
@@ -2732,7 +2732,7 @@
         <v>181</v>
       </c>
       <c r="C28" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D28" s="3">
         <v>54</v>
@@ -2744,7 +2744,7 @@
         <v>95</v>
       </c>
       <c r="G28" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H28" s="3">
         <v>26</v>
@@ -2764,7 +2764,7 @@
       <c r="O28" s="3"/>
       <c r="P28">
         <f t="shared" si="7"/>
-        <v>608</v>
+        <v>703</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="9"/>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="R28" t="str">
         <f t="shared" si="10"/>
-        <v>{1400, 30}</v>
+        <v>{1400, 45}</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="11"/>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="V28" t="str">
         <f t="shared" si="2"/>
-        <v>{1400, 20}</v>
+        <v>{1400, 100}</v>
       </c>
       <c r="W28" t="str">
         <f t="shared" si="3"/>
@@ -2815,7 +2815,7 @@
         <v>182</v>
       </c>
       <c r="C29" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D29" s="4">
         <v>58</v>
@@ -2827,7 +2827,7 @@
         <v>102</v>
       </c>
       <c r="G29" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H29" s="3">
         <v>26</v>
@@ -2847,7 +2847,7 @@
       <c r="O29" s="3"/>
       <c r="P29">
         <f t="shared" si="7"/>
-        <v>625</v>
+        <v>720</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="9"/>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="R29" t="str">
         <f t="shared" si="10"/>
-        <v>{1500, 30}</v>
+        <v>{1500, 45}</v>
       </c>
       <c r="S29" t="str">
         <f t="shared" si="11"/>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="V29" t="str">
         <f t="shared" si="2"/>
-        <v>{1500, 20}</v>
+        <v>{1500, 100}</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="3"/>
@@ -2898,7 +2898,7 @@
         <v>183</v>
       </c>
       <c r="C30" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D30" s="3">
         <v>62</v>
@@ -2910,7 +2910,7 @@
         <v>109</v>
       </c>
       <c r="G30" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H30" s="3">
         <v>26</v>
@@ -2930,7 +2930,7 @@
       <c r="O30" s="3"/>
       <c r="P30">
         <f t="shared" si="7"/>
-        <v>642</v>
+        <v>737</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="9"/>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="R30" t="str">
         <f t="shared" si="10"/>
-        <v>{1600, 30}</v>
+        <v>{1600, 45}</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" si="11"/>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="V30" t="str">
         <f t="shared" si="2"/>
-        <v>{1600, 20}</v>
+        <v>{1600, 100}</v>
       </c>
       <c r="W30" t="str">
         <f t="shared" si="3"/>
@@ -2981,7 +2981,7 @@
         <v>184</v>
       </c>
       <c r="C31" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D31" s="4">
         <v>66</v>
@@ -2993,7 +2993,7 @@
         <v>116</v>
       </c>
       <c r="G31" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H31" s="3">
         <v>26</v>
@@ -3013,7 +3013,7 @@
       <c r="O31" s="3"/>
       <c r="P31">
         <f t="shared" si="7"/>
-        <v>659</v>
+        <v>754</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="9"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="R31" t="str">
         <f t="shared" si="10"/>
-        <v>{1700, 30}</v>
+        <v>{1700, 45}</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="11"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="V31" t="str">
         <f t="shared" si="2"/>
-        <v>{1700, 20}</v>
+        <v>{1700, 100}</v>
       </c>
       <c r="W31" t="str">
         <f t="shared" si="3"/>
@@ -3064,7 +3064,7 @@
         <v>185</v>
       </c>
       <c r="C32" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D32" s="3">
         <v>70</v>
@@ -3076,7 +3076,7 @@
         <v>123</v>
       </c>
       <c r="G32" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H32" s="3">
         <v>26</v>
@@ -3096,7 +3096,7 @@
       <c r="O32" s="3"/>
       <c r="P32">
         <f t="shared" si="7"/>
-        <v>676</v>
+        <v>771</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="9"/>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="R32" t="str">
         <f t="shared" si="10"/>
-        <v>{1800, 30}</v>
+        <v>{1800, 45}</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="11"/>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="V32" t="str">
         <f t="shared" si="2"/>
-        <v>{1800, 20}</v>
+        <v>{1800, 100}</v>
       </c>
       <c r="W32" t="str">
         <f t="shared" si="3"/>
@@ -3147,7 +3147,7 @@
         <v>186</v>
       </c>
       <c r="C33" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D33" s="4">
         <v>74</v>
@@ -3179,7 +3179,7 @@
       <c r="O33" s="3"/>
       <c r="P33">
         <f t="shared" si="7"/>
-        <v>693</v>
+        <v>708</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="9"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="R33" t="str">
         <f t="shared" si="10"/>
-        <v>{1900, 30}</v>
+        <v>{1900, 45}</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="11"/>
@@ -3230,7 +3230,7 @@
         <v>187</v>
       </c>
       <c r="C34" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D34" s="3">
         <v>78</v>
@@ -3262,7 +3262,7 @@
       <c r="O34" s="3"/>
       <c r="P34">
         <f t="shared" si="7"/>
-        <v>710</v>
+        <v>725</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="9"/>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="R34" t="str">
         <f t="shared" si="10"/>
-        <v>{2000, 30}</v>
+        <v>{2000, 45}</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="11"/>
@@ -3313,7 +3313,7 @@
         <v>188</v>
       </c>
       <c r="C35" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D35" s="4">
         <v>82</v>
@@ -3345,7 +3345,7 @@
       <c r="O35" s="3"/>
       <c r="P35">
         <f t="shared" si="7"/>
-        <v>727</v>
+        <v>742</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" si="9"/>
@@ -3353,7 +3353,7 @@
       </c>
       <c r="R35" t="str">
         <f t="shared" si="10"/>
-        <v>{2250, 30}</v>
+        <v>{2250, 45}</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="11"/>
@@ -3396,7 +3396,7 @@
         <v>189</v>
       </c>
       <c r="C36" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D36" s="3">
         <v>86</v>
@@ -3428,7 +3428,7 @@
       <c r="O36" s="3"/>
       <c r="P36">
         <f t="shared" si="7"/>
-        <v>744</v>
+        <v>759</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" si="9"/>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="R36" t="str">
         <f t="shared" si="10"/>
-        <v>{2500, 30}</v>
+        <v>{2500, 45}</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" si="11"/>
@@ -3479,7 +3479,7 @@
         <v>190</v>
       </c>
       <c r="C37" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4">
         <v>90</v>
@@ -3511,7 +3511,7 @@
       <c r="O37" s="3"/>
       <c r="P37">
         <f t="shared" si="7"/>
-        <v>761</v>
+        <v>776</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" si="9"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="R37" t="str">
         <f t="shared" si="10"/>
-        <v>{2750, 30}</v>
+        <v>{2750, 45}</v>
       </c>
       <c r="S37" t="str">
         <f t="shared" si="11"/>
@@ -3562,7 +3562,7 @@
         <v>191</v>
       </c>
       <c r="C38" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D38" s="3">
         <v>94</v>
@@ -3594,7 +3594,7 @@
       <c r="O38" s="3"/>
       <c r="P38">
         <f t="shared" si="7"/>
-        <v>778</v>
+        <v>793</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" si="9"/>
@@ -3602,7 +3602,7 @@
       </c>
       <c r="R38" t="str">
         <f t="shared" si="10"/>
-        <v>{3000, 30}</v>
+        <v>{3000, 45}</v>
       </c>
       <c r="S38" t="str">
         <f t="shared" si="11"/>
@@ -3645,7 +3645,7 @@
         <v>192</v>
       </c>
       <c r="C39" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D39" s="4">
         <v>98</v>
@@ -3677,7 +3677,7 @@
       <c r="O39" s="3"/>
       <c r="P39">
         <f>SUM(B39:O39)</f>
-        <v>795</v>
+        <v>810</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" si="9"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="R39" t="str">
         <f t="shared" si="10"/>
-        <v>{3250, 30}</v>
+        <v>{3250, 45}</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" si="11"/>
@@ -3728,7 +3728,7 @@
         <v>193</v>
       </c>
       <c r="C40" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D40" s="3">
         <v>102</v>
@@ -3737,7 +3737,7 @@
         <v>135</v>
       </c>
       <c r="F40" s="3">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="G40" s="3">
         <v>20</v>
@@ -3760,7 +3760,7 @@
       <c r="O40" s="3"/>
       <c r="P40">
         <f t="shared" si="7"/>
-        <v>812</v>
+        <v>898</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" si="9"/>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="R40" t="str">
         <f t="shared" si="10"/>
-        <v>{3500, 30}</v>
+        <v>{3500, 45}</v>
       </c>
       <c r="S40" t="str">
         <f t="shared" si="11"/>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="U40" t="str">
         <f t="shared" si="13"/>
-        <v>{3500, 179}</v>
+        <v>{3500, 250}</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" si="2"/>
@@ -3868,11 +3868,11 @@
       </c>
       <c r="B46" t="str">
         <f>CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", Q2:Q39),"}")</f>
-        <v>{{0, 10}, {10, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {850, 170}, {900, 171}, {950, 172}, {1000, 173}, {1050, 174}, {1100, 175}, {1150, 176}, {1200, 177}, {1250, 178}, {1300, 179}, {1350, 180}, {1400, 181}, {1500, 182}, {1600, 183}, {1700, 184}, {1800, 185}, {1900, 186}, {2000, 187}, {2250, 188}, {2500, 189}, {2750, 190}, {3000, 191}, {3250, 192}}</v>
+        <v>{{0, 80}, {10, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {850, 170}, {900, 171}, {950, 172}, {1000, 173}, {1050, 174}, {1100, 175}, {1150, 176}, {1200, 177}, {1250, 178}, {1300, 179}, {1350, 180}, {1400, 181}, {1500, 182}, {1600, 183}, {1700, 184}, {1800, 185}, {1900, 186}, {2000, 187}, {2250, 188}, {2500, 189}, {2750, 190}, {3000, 191}, {3250, 192}}</v>
       </c>
       <c r="C46" t="str">
         <f>CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", R2:R39),"}")</f>
-        <v>{{0, 50}, {10, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 40}, {750, 35}, {800, 30}, {850, 30}, {900, 30}, {950, 30}, {1000, 30}, {1050, 30}, {1100, 30}, {1150, 30}, {1200, 30}, {1250, 30}, {1300, 30}, {1350, 30}, {1400, 30}, {1500, 30}, {1600, 30}, {1700, 30}, {1800, 30}, {1900, 30}, {2000, 30}, {2250, 30}, {2500, 30}, {2750, 30}, {3000, 30}, {3250, 30}}</v>
+        <v>{{0, 90}, {10, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 45}, {750, 45}, {800, 45}, {850, 45}, {900, 45}, {950, 45}, {1000, 45}, {1050, 45}, {1100, 45}, {1150, 45}, {1200, 45}, {1250, 45}, {1300, 45}, {1350, 45}, {1400, 45}, {1500, 45}, {1600, 45}, {1700, 45}, {1800, 45}, {1900, 45}, {2000, 45}, {2250, 45}, {2500, 45}, {2750, 45}, {3000, 45}, {3250, 45}}</v>
       </c>
       <c r="D46" t="str">
         <f>CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", S2:S39),"}")</f>
@@ -3884,15 +3884,15 @@
       </c>
       <c r="F46" t="str">
         <f>CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", U2:U39),"}")</f>
-        <v>{{0, 0}, {10, 1}, {200, 1}, {250, 18}, {300, 18}, {350, 18}, {400, 18}, {450, 18}, {500, 18}, {550, 18}, {600, 18}, {650, 18}, {700, 18}, {750, 18}, {800, 18}, {850, 18}, {900, 25}, {950, 32}, {1000, 39}, {1050, 46}, {1100, 53}, {1150, 60}, {1200, 67}, {1250, 74}, {1300, 81}, {1350, 88}, {1400, 95}, {1500, 102}, {1600, 109}, {1700, 116}, {1800, 123}, {1900, 130}, {2000, 137}, {2250, 144}, {2500, 151}, {2750, 158}, {3000, 165}, {3250, 172}}</v>
+        <v>{{0, 0}, {10, 1}, {200, 1}, {250, 18}, {300, 18}, {350, 18}, {400, 18}, {450, 18}, {500, 18}, {550, 18}, {600, 18}, {650, 50}, {700, 50}, {750, 50}, {800, 50}, {850, 50}, {900, 50}, {950, 50}, {1000, 50}, {1050, 50}, {1100, 53}, {1150, 60}, {1200, 67}, {1250, 74}, {1300, 81}, {1350, 88}, {1400, 95}, {1500, 102}, {1600, 109}, {1700, 116}, {1800, 123}, {1900, 130}, {2000, 137}, {2250, 144}, {2500, 151}, {2750, 158}, {3000, 165}, {3250, 172}}</v>
       </c>
       <c r="G46" s="2" t="str">
         <f t="shared" ref="G46:N46" si="15">CONCATENATE("{",_xlfn.TEXTJOIN(", ","FALSCH", V2:V17),"}")</f>
-        <v>{{0, 2}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 80}, {400, 10}, {450, 50}, {500, 10}, {550, 100}, {600, 20}, {650, 20}, {700, 20}, {750, 20}, {800, 20}, {850, 20}}</v>
+        <v>{{0, 20}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 80}, {400, 10}, {450, 50}, {500, 10}, {550, 100}, {600, 100}, {650, 100}, {700, 100}, {750, 100}, {800, 20}, {850, 20}}</v>
       </c>
       <c r="H46" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{{0, 2}, {10, 10}, {200, 18}, {250, 26}, {300, 26}, {350, 26}, {400, 26}, {450, 26}, {500, 26}, {550, 26}, {600, 26}, {650, 26}, {700, 26}, {750, 26}, {800, 26}, {850, 26}}</v>
+        <v>{{0, 20}, {10, 10}, {200, 18}, {250, 26}, {300, 26}, {350, 26}, {400, 26}, {450, 26}, {500, 26}, {550, 26}, {600, 26}, {650, 26}, {700, 26}, {750, 26}, {800, 26}, {850, 26}}</v>
       </c>
       <c r="I46" s="2" t="str">
         <f t="shared" si="15"/>
@@ -3900,11 +3900,11 @@
       </c>
       <c r="J46" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{{0, 0}, {10, 2}, {200, 1}, {250, 1}, {300, 1}, {350, 1}, {400, 1}, {450, 1}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}}</v>
+        <v>{{0, 5}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 10}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}}</v>
       </c>
       <c r="K46" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{{0, 0}, {10, 10}, {200, 1}, {250, 1}, {300, 1}, {350, 1}, {400, 1}, {450, 1}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}}</v>
+        <v>{{0, 5}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 10}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}}</v>
       </c>
       <c r="L46" s="2" t="str">
         <f t="shared" si="15"/>
@@ -3923,11 +3923,11 @@
       <c r="A49" s="1"/>
       <c r="B49" t="str">
         <f>CONCATENATE("private static readonly Dictionary&lt;int, float&gt; ",B1,"SpawnProbabilities = new Dictionary&lt;int, float&gt;  ", B46,";")</f>
-        <v>private static readonly Dictionary&lt;int, float&gt; CoinSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 10}, {10, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {850, 170}, {900, 171}, {950, 172}, {1000, 173}, {1050, 174}, {1100, 175}, {1150, 176}, {1200, 177}, {1250, 178}, {1300, 179}, {1350, 180}, {1400, 181}, {1500, 182}, {1600, 183}, {1700, 184}, {1800, 185}, {1900, 186}, {2000, 187}, {2250, 188}, {2500, 189}, {2750, 190}, {3000, 191}, {3250, 192}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; CoinSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 80}, {10, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {850, 170}, {900, 171}, {950, 172}, {1000, 173}, {1050, 174}, {1100, 175}, {1150, 176}, {1200, 177}, {1250, 178}, {1300, 179}, {1350, 180}, {1400, 181}, {1500, 182}, {1600, 183}, {1700, 184}, {1800, 185}, {1900, 186}, {2000, 187}, {2250, 188}, {2500, 189}, {2750, 190}, {3000, 191}, {3250, 192}};</v>
       </c>
       <c r="C49" t="str">
         <f>CONCATENATE("private static readonly Dictionary&lt;int, float&gt; ",C1,"SpawnProbabilities = new Dictionary&lt;int, float&gt;  ", C46,";")</f>
-        <v>private static readonly Dictionary&lt;int, float&gt; BananaSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 50}, {10, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 40}, {750, 35}, {800, 30}, {850, 30}, {900, 30}, {950, 30}, {1000, 30}, {1050, 30}, {1100, 30}, {1150, 30}, {1200, 30}, {1250, 30}, {1300, 30}, {1350, 30}, {1400, 30}, {1500, 30}, {1600, 30}, {1700, 30}, {1800, 30}, {1900, 30}, {2000, 30}, {2250, 30}, {2500, 30}, {2750, 30}, {3000, 30}, {3250, 30}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; BananaSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 90}, {10, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 45}, {750, 45}, {800, 45}, {850, 45}, {900, 45}, {950, 45}, {1000, 45}, {1050, 45}, {1100, 45}, {1150, 45}, {1200, 45}, {1250, 45}, {1300, 45}, {1350, 45}, {1400, 45}, {1500, 45}, {1600, 45}, {1700, 45}, {1800, 45}, {1900, 45}, {2000, 45}, {2250, 45}, {2500, 45}, {2750, 45}, {3000, 45}, {3250, 45}};</v>
       </c>
       <c r="D49" t="str">
         <f>CONCATENATE("private static readonly Dictionary&lt;int, float&gt; ",D1,"SpawnProbabilities = new Dictionary&lt;int, float&gt;  ", D46,";")</f>
@@ -3939,15 +3939,15 @@
       </c>
       <c r="F49" t="str">
         <f>CONCATENATE("private static readonly Dictionary&lt;int, float&gt; ",F1,"SpawnProbabilities = new Dictionary&lt;int, float&gt;  ", F46,";")</f>
-        <v>private static readonly Dictionary&lt;int, float&gt; RedShelliSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 1}, {200, 1}, {250, 18}, {300, 18}, {350, 18}, {400, 18}, {450, 18}, {500, 18}, {550, 18}, {600, 18}, {650, 18}, {700, 18}, {750, 18}, {800, 18}, {850, 18}, {900, 25}, {950, 32}, {1000, 39}, {1050, 46}, {1100, 53}, {1150, 60}, {1200, 67}, {1250, 74}, {1300, 81}, {1350, 88}, {1400, 95}, {1500, 102}, {1600, 109}, {1700, 116}, {1800, 123}, {1900, 130}, {2000, 137}, {2250, 144}, {2500, 151}, {2750, 158}, {3000, 165}, {3250, 172}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; RedShelliSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 1}, {200, 1}, {250, 18}, {300, 18}, {350, 18}, {400, 18}, {450, 18}, {500, 18}, {550, 18}, {600, 18}, {650, 50}, {700, 50}, {750, 50}, {800, 50}, {850, 50}, {900, 50}, {950, 50}, {1000, 50}, {1050, 50}, {1100, 53}, {1150, 60}, {1200, 67}, {1250, 74}, {1300, 81}, {1350, 88}, {1400, 95}, {1500, 102}, {1600, 109}, {1700, 116}, {1800, 123}, {1900, 130}, {2000, 137}, {2250, 144}, {2500, 151}, {2750, 158}, {3000, 165}, {3250, 172}};</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" ref="G49:K49" si="16">CONCATENATE("private static readonly Dictionary&lt;int, float&gt; ",G1,"SpawnProbabilities = new Dictionary&lt;int, float&gt;  ", G46,";")</f>
-        <v>private static readonly Dictionary&lt;int, float&gt; FlashiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 2}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 80}, {400, 10}, {450, 50}, {500, 10}, {550, 100}, {600, 20}, {650, 20}, {700, 20}, {750, 20}, {800, 20}, {850, 20}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; FlashiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 20}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 80}, {400, 10}, {450, 50}, {500, 10}, {550, 100}, {600, 100}, {650, 100}, {700, 100}, {750, 100}, {800, 20}, {850, 20}};</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="16"/>
-        <v>private static readonly Dictionary&lt;int, float&gt; GhostiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 2}, {10, 10}, {200, 18}, {250, 26}, {300, 26}, {350, 26}, {400, 26}, {450, 26}, {500, 26}, {550, 26}, {600, 26}, {650, 26}, {700, 26}, {750, 26}, {800, 26}, {850, 26}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; GhostiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 20}, {10, 10}, {200, 18}, {250, 26}, {300, 26}, {350, 26}, {400, 26}, {450, 26}, {500, 26}, {550, 26}, {600, 26}, {650, 26}, {700, 26}, {750, 26}, {800, 26}, {850, 26}};</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="16"/>
@@ -3955,26 +3955,26 @@
       </c>
       <c r="J49" t="str">
         <f t="shared" si="16"/>
-        <v>private static readonly Dictionary&lt;int, float&gt; RockiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 2}, {200, 1}, {250, 1}, {300, 1}, {350, 1}, {400, 1}, {450, 1}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; RockiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 5}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 10}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="16"/>
-        <v>private static readonly Dictionary&lt;int, float&gt; StariSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 10}, {200, 1}, {250, 1}, {300, 1}, {350, 1}, {400, 1}, {450, 1}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};</v>
+        <v>private static readonly Dictionary&lt;int, float&gt; StariSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 5}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 10}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="5" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(10), FALSE,B49:N49)</f>
-        <v xml:space="preserve">private static readonly Dictionary&lt;int, float&gt; CoinSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 10}, {10, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {850, 170}, {900, 171}, {950, 172}, {1000, 173}, {1050, 174}, {1100, 175}, {1150, 176}, {1200, 177}, {1250, 178}, {1300, 179}, {1350, 180}, {1400, 181}, {1500, 182}, {1600, 183}, {1700, 184}, {1800, 185}, {1900, 186}, {2000, 187}, {2250, 188}, {2500, 189}, {2750, 190}, {3000, 191}, {3250, 192}};
-private static readonly Dictionary&lt;int, float&gt; BananaSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 50}, {10, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 40}, {750, 35}, {800, 30}, {850, 30}, {900, 30}, {950, 30}, {1000, 30}, {1050, 30}, {1100, 30}, {1150, 30}, {1200, 30}, {1250, 30}, {1300, 30}, {1350, 30}, {1400, 30}, {1500, 30}, {1600, 30}, {1700, 30}, {1800, 30}, {1900, 30}, {2000, 30}, {2250, 30}, {2500, 30}, {2750, 30}, {3000, 30}, {3250, 30}};
+        <v xml:space="preserve">private static readonly Dictionary&lt;int, float&gt; CoinSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 80}, {10, 105}, {200, 110}, {250, 115}, {300, 120}, {350, 125}, {400, 130}, {450, 135}, {500, 140}, {550, 145}, {600, 150}, {650, 155}, {700, 160}, {750, 165}, {800, 170}, {850, 170}, {900, 171}, {950, 172}, {1000, 173}, {1050, 174}, {1100, 175}, {1150, 176}, {1200, 177}, {1250, 178}, {1300, 179}, {1350, 180}, {1400, 181}, {1500, 182}, {1600, 183}, {1700, 184}, {1800, 185}, {1900, 186}, {2000, 187}, {2250, 188}, {2500, 189}, {2750, 190}, {3000, 191}, {3250, 192}};
+private static readonly Dictionary&lt;int, float&gt; BananaSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 90}, {10, 95}, {200, 90}, {250, 85}, {300, 80}, {350, 75}, {400, 70}, {450, 65}, {500, 60}, {550, 55}, {600, 50}, {650, 45}, {700, 45}, {750, 45}, {800, 45}, {850, 45}, {900, 45}, {950, 45}, {1000, 45}, {1050, 45}, {1100, 45}, {1150, 45}, {1200, 45}, {1250, 45}, {1300, 45}, {1350, 45}, {1400, 45}, {1500, 45}, {1600, 45}, {1700, 45}, {1800, 45}, {1900, 45}, {2000, 45}, {2250, 45}, {2500, 45}, {2750, 45}, {3000, 45}, {3250, 45}};
 private static readonly Dictionary&lt;int, float&gt; BlueShelliSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 0}, {200, 0}, {250, 0}, {300, 0}, {350, 0}, {400, 10}, {450, 12}, {500, 14}, {550, 16}, {600, 18}, {650, 20}, {700, 22}, {750, 24}, {800, 26}, {850, 28}, {900, 30}, {950, 32}, {1000, 34}, {1050, 36}, {1100, 38}, {1150, 40}, {1200, 42}, {1250, 44}, {1300, 46}, {1350, 50}, {1400, 54}, {1500, 58}, {1600, 62}, {1700, 66}, {1800, 70}, {1900, 74}, {2000, 78}, {2250, 82}, {2500, 86}, {2750, 90}, {3000, 94}, {3250, 98}};
 private static readonly Dictionary&lt;int, float&gt; GreenShelliSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 5}, {10, 5}, {200, 5}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 20}, {500, 40}, {550, 40}, {600, 40}, {650, 20}, {700, 20}, {750, 20}, {800, 20}, {850, 20}, {900, 25}, {950, 30}, {1000, 35}, {1050, 40}, {1100, 45}, {1150, 50}, {1200, 55}, {1250, 60}, {1300, 65}, {1350, 70}, {1400, 75}, {1500, 80}, {1600, 85}, {1700, 90}, {1800, 95}, {1900, 100}, {2000, 105}, {2250, 110}, {2500, 115}, {2750, 120}, {3000, 125}, {3250, 130}};
-private static readonly Dictionary&lt;int, float&gt; RedShelliSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 1}, {200, 1}, {250, 18}, {300, 18}, {350, 18}, {400, 18}, {450, 18}, {500, 18}, {550, 18}, {600, 18}, {650, 18}, {700, 18}, {750, 18}, {800, 18}, {850, 18}, {900, 25}, {950, 32}, {1000, 39}, {1050, 46}, {1100, 53}, {1150, 60}, {1200, 67}, {1250, 74}, {1300, 81}, {1350, 88}, {1400, 95}, {1500, 102}, {1600, 109}, {1700, 116}, {1800, 123}, {1900, 130}, {2000, 137}, {2250, 144}, {2500, 151}, {2750, 158}, {3000, 165}, {3250, 172}};
-private static readonly Dictionary&lt;int, float&gt; FlashiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 2}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 80}, {400, 10}, {450, 50}, {500, 10}, {550, 100}, {600, 20}, {650, 20}, {700, 20}, {750, 20}, {800, 20}, {850, 20}};
-private static readonly Dictionary&lt;int, float&gt; GhostiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 2}, {10, 10}, {200, 18}, {250, 26}, {300, 26}, {350, 26}, {400, 26}, {450, 26}, {500, 26}, {550, 26}, {600, 26}, {650, 26}, {700, 26}, {750, 26}, {800, 26}, {850, 26}};
+private static readonly Dictionary&lt;int, float&gt; RedShelliSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 1}, {200, 1}, {250, 18}, {300, 18}, {350, 18}, {400, 18}, {450, 18}, {500, 18}, {550, 18}, {600, 18}, {650, 50}, {700, 50}, {750, 50}, {800, 50}, {850, 50}, {900, 50}, {950, 50}, {1000, 50}, {1050, 50}, {1100, 53}, {1150, 60}, {1200, 67}, {1250, 74}, {1300, 81}, {1350, 88}, {1400, 95}, {1500, 102}, {1600, 109}, {1700, 116}, {1800, 123}, {1900, 130}, {2000, 137}, {2250, 144}, {2500, 151}, {2750, 158}, {3000, 165}, {3250, 172}};
+private static readonly Dictionary&lt;int, float&gt; FlashiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 20}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 80}, {400, 10}, {450, 50}, {500, 10}, {550, 100}, {600, 100}, {650, 100}, {700, 100}, {750, 100}, {800, 20}, {850, 20}};
+private static readonly Dictionary&lt;int, float&gt; GhostiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 20}, {10, 10}, {200, 18}, {250, 26}, {300, 26}, {350, 26}, {400, 26}, {450, 26}, {500, 26}, {550, 26}, {600, 26}, {650, 26}, {700, 26}, {750, 26}, {800, 26}, {850, 26}};
 private static readonly Dictionary&lt;int, float&gt; MushiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 1}, {10, 20}, {200, 39}, {250, 58}, {300, 58}, {350, 58}, {400, 58}, {450, 58}, {500, 58}, {550, 58}, {600, 58}, {650, 58}, {700, 58}, {750, 58}, {800, 77}, {850, 77}};
-private static readonly Dictionary&lt;int, float&gt; RockiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 2}, {200, 1}, {250, 1}, {300, 1}, {350, 1}, {400, 1}, {450, 1}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};
-private static readonly Dictionary&lt;int, float&gt; StariSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 0}, {10, 10}, {200, 1}, {250, 1}, {300, 1}, {350, 1}, {400, 1}, {450, 1}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};
+private static readonly Dictionary&lt;int, float&gt; RockiSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 5}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 10}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};
+private static readonly Dictionary&lt;int, float&gt; StariSpawnProbabilities = new Dictionary&lt;int, float&gt;  {{0, 5}, {10, 10}, {200, 10}, {250, 10}, {300, 10}, {350, 10}, {400, 10}, {450, 10}, {500, 25}, {550, 25}, {600, 25}, {650, 25}, {700, 25}, {750, 25}, {800, 25}, {850, 25}};
 </v>
       </c>
     </row>

</xml_diff>